<commit_message>
exp1. with proper decay group!
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gaohn/learning-agency-lab-automated-essay-scoring-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/omniverse/learning-agency-lab-automated-essay-scoring-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E599FB-5E75-5D44-BE9C-61458D7339FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB50370-EC56-9142-B7F3-92AAC808197B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="21100" activeTab="1" xr2:uid="{78DCD112-02ED-B440-9BA7-48C6A208E221}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21100" activeTab="1" xr2:uid="{78DCD112-02ED-B440-9BA7-48C6A208E221}"/>
   </bookViews>
   <sheets>
     <sheet name="exp" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">exp!$A$1:$S$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="70">
   <si>
     <t>run name</t>
   </si>
@@ -226,6 +225,27 @@
   </si>
   <si>
     <t>1536/1536</t>
+  </si>
+  <si>
+    <t>c62429ece4a9ac7417a635f5932dae136bdd8f6d</t>
+  </si>
+  <si>
+    <t>v20240628210409</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>reinitialize_n_layers_of_backbone</t>
+  </si>
+  <si>
+    <t>llrd</t>
+  </si>
+  <si>
+    <t>adamw-forgot-wd</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1111,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="A2" sqref="A2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1985,12 +2005,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401DFEB0-8383-2943-9F78-E4FE25E99B51}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="88.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <v>20230310</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor edits to docs
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gaohn/learning-agency-lab-automated-essay-scoring-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B69AFA8-64E7-B442-B864-149A4654BDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F74B7-501D-0A40-8C65-20CC96626BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="21100" activeTab="1" xr2:uid="{78DCD112-02ED-B440-9BA7-48C6A208E221}"/>
   </bookViews>
@@ -815,7 +815,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -830,6 +830,9 @@
     </xf>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1740,7 +1743,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3277,6 +3280,9 @@
         <v>54</v>
       </c>
     </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+    </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G30" s="1"/>
       <c r="H30"/>

</xml_diff>